<commit_message>
add all the UW
</commit_message>
<xml_diff>
--- a/DataSheet/FOS5_Till_UW.xlsx
+++ b/DataSheet/FOS5_Till_UW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F003C2-8BC1-4173-A178-4EF993C88497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895E988B-CB1B-4259-AE59-FBB84538857E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4113" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="573">
   <si>
     <t>Si_No</t>
   </si>
@@ -2264,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O400"/>
+  <dimension ref="A1:O401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="74" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="74" workbookViewId="0">
+      <selection activeCell="H401" sqref="H401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15147,6 +15147,26 @@
       </c>
       <c r="O400" t="s">
         <v>291</v>
+      </c>
+    </row>
+    <row r="401" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A401" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B401" t="s">
+        <v>15</v>
+      </c>
+      <c r="C401" t="s">
+        <v>276</v>
+      </c>
+      <c r="D401" t="s">
+        <v>16</v>
+      </c>
+      <c r="H401" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O401" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started cpc 1 touch point and add a new scrool function class because of mobile and web scroll it is not working ate same class
</commit_message>
<xml_diff>
--- a/DataSheet/FOS5_Till_UW.xlsx
+++ b/DataSheet/FOS5_Till_UW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895E988B-CB1B-4259-AE59-FBB84538857E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FC9BF1-CD1D-4F33-A22C-84FAFE1635B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2266,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="74" workbookViewId="0">
-      <selection activeCell="H401" sqref="H401"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="74" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15180,8 +15180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="AD1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15369,16 +15369,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2" t="s">
         <v>174</v>
@@ -15387,7 +15387,7 @@
         <v>232</v>
       </c>
       <c r="L2" s="8">
-        <v>45698</v>
+        <v>46063</v>
       </c>
       <c r="M2" t="s">
         <v>240</v>
@@ -15450,13 +15450,13 @@
         <v>519</v>
       </c>
       <c r="AG2">
-        <v>7978067010</v>
+        <v>9937762834</v>
       </c>
       <c r="AH2" t="s">
         <v>524</v>
       </c>
       <c r="AI2">
-        <v>7744008734</v>
+        <v>9937949551</v>
       </c>
       <c r="AJ2" t="s">
         <v>531</v>

</xml_diff>